<commit_message>
modify deepops guide docs
</commit_message>
<xml_diff>
--- a/deepops/DeepOps_version_list.xlsx
+++ b/deepops/DeepOps_version_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kb01-jjsair0412/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kb01-jjsair0412/kubernetes_info/deepops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6EAACF-111D-1F40-AF49-E013C9CFAC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA94C909-F682-7A4E-84E9-554083B93B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5140" yWindow="2280" windowWidth="28300" windowHeight="17440" xr2:uid="{6100C474-37A7-464C-A1B9-E018EC4BCF0B}"/>
   </bookViews>
@@ -422,28 +422,28 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -763,7 +763,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G18"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -773,15 +773,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="22">
       <c r="A3" s="2" t="s">
@@ -953,7 +953,7 @@
       <c r="E11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="11">
         <v>20.02</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -970,7 +970,7 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1">
@@ -1070,7 +1070,7 @@
       <c r="F17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="13" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       <c r="F18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1">
       <c r="A19" s="3">
@@ -1127,16 +1127,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="G17:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>